<commit_message>
update new orleans xlsx files
</commit_message>
<xml_diff>
--- a/data/hotels_by_city/New_Orleans/Tripadvisor_new_orleans_shard_100.xlsx
+++ b/data/hotels_by_city/New_Orleans/Tripadvisor_new_orleans_shard_100.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="hotel_info" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="review_info" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="review_info" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="hotel_info" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,14 +16,89 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
   <si>
     <t>STR</t>
   </si>
   <si>
+    <t>reviewer_ID</t>
+  </si>
+  <si>
+    <t>reviewer_name</t>
+  </si>
+  <si>
+    <t>Review_ID</t>
+  </si>
+  <si>
+    <t>Date_of_scraping</t>
+  </si>
+  <si>
+    <t>ReviewURL</t>
+  </si>
+  <si>
+    <t>Tripadvisor_gcode</t>
+  </si>
+  <si>
+    <t>Tripadvisor_dcode</t>
+  </si>
+  <si>
+    <t>Tripadvisor_rcode</t>
+  </si>
+  <si>
+    <t>review_date</t>
+  </si>
+  <si>
+    <t>review_title</t>
+  </si>
+  <si>
+    <t>review_content</t>
+  </si>
+  <si>
+    <t>review_rating</t>
+  </si>
+  <si>
+    <t>trip_month</t>
+  </si>
+  <si>
+    <t>trip_purpose</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>rooms</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Cleanliness</t>
+  </si>
+  <si>
+    <t>Sleep Quality</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Picture(yes=1)</t>
+  </si>
+  <si>
+    <t>respondent</t>
+  </si>
+  <si>
+    <t>response_date</t>
+  </si>
+  <si>
+    <t>response_text</t>
+  </si>
+  <si>
     <t>Hotel_Name</t>
   </si>
   <si>
+    <t>State</t>
+  </si>
+  <si>
     <t>City</t>
   </si>
   <si>
@@ -48,6 +123,9 @@
     <t>Holiday Inn New Orleans Downtown Superdome</t>
   </si>
   <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
     <t>New Orleans</t>
   </si>
   <si>
@@ -64,78 +142,6 @@
   </si>
   <si>
     <t>1309</t>
-  </si>
-  <si>
-    <t>reviewer_ID</t>
-  </si>
-  <si>
-    <t>reviewer_name</t>
-  </si>
-  <si>
-    <t>Review_ID</t>
-  </si>
-  <si>
-    <t>Date_of_scraping</t>
-  </si>
-  <si>
-    <t>ReviewURL</t>
-  </si>
-  <si>
-    <t>Tripadvisor_gcode</t>
-  </si>
-  <si>
-    <t>Tripadvisor_dcode</t>
-  </si>
-  <si>
-    <t>Tripadvisor_rcode</t>
-  </si>
-  <si>
-    <t>review_date</t>
-  </si>
-  <si>
-    <t>review_title</t>
-  </si>
-  <si>
-    <t>review_content</t>
-  </si>
-  <si>
-    <t>review_rating</t>
-  </si>
-  <si>
-    <t>trip_month</t>
-  </si>
-  <si>
-    <t>trip_purpose</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>rooms</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Cleanliness</t>
-  </si>
-  <si>
-    <t>Sleep Quality</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>Picture(yes=1)</t>
-  </si>
-  <si>
-    <t>respondent</t>
-  </si>
-  <si>
-    <t>response_date</t>
-  </si>
-  <si>
-    <t>response_text</t>
   </si>
 </sst>
 </file>
@@ -506,34 +512,53 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>4351</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="n">
-        <v>70112</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="I2" t="s">
+      <c r="P1" t="s">
         <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -558,76 +583,63 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>31</v>
-      </c>
-      <c r="R1" t="s">
-        <v>32</v>
-      </c>
-      <c r="S1" t="s">
         <v>33</v>
       </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>4351</v>
+      </c>
+      <c r="B2" t="s">
         <v>34</v>
       </c>
-      <c r="U1" t="s">
+      <c r="C2" t="s">
         <v>35</v>
       </c>
-      <c r="V1" t="s">
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="W1" t="s">
+      <c r="E2" t="n">
+        <v>70112</v>
+      </c>
+      <c r="F2" t="s">
         <v>37</v>
       </c>
-      <c r="X1" t="s">
+      <c r="G2" t="s">
         <v>38</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="H2" t="s">
         <v>39</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>